<commit_message>
report basically done, profiling done
</commit_message>
<xml_diff>
--- a/24c - Spike - Performance Measurement/Spike 24 results.xlsx
+++ b/24c - Spike - Performance Measurement/Spike 24 results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\benho\Documents\Uni-Work\COS30031-103024841\24c - Spike - Performance Measurement\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67C5A4BD-86B4-48EF-AFB6-71D2D74190B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D2ED265-0BE9-4BDB-972E-13C09125160A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{1384FB0F-FE1E-4D09-AAC5-4719FCE4A392}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="16">
   <si>
     <t>File size 100</t>
   </si>
@@ -84,6 +84,9 @@
   </si>
   <si>
     <t>release file 1000</t>
+  </si>
+  <si>
+    <t>percent change</t>
   </si>
 </sst>
 </file>
@@ -657,7 +660,7 @@
                 </a:r>
                 <a:r>
                   <a:rPr lang="en-AU" baseline="0"/>
-                  <a:t> (milliseconds)</a:t>
+                  <a:t> (microseconds)</a:t>
                 </a:r>
                 <a:endParaRPr lang="en-AU"/>
               </a:p>
@@ -902,7 +905,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Scalability!$I$3</c:f>
+              <c:f>Scalability!$A$21</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -923,7 +926,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Scalability!$J$2:$L$2</c:f>
+              <c:f>Scalability!$B$20:$D$20</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -940,7 +943,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Scalability!$J$3:$L$3</c:f>
+              <c:f>Scalability!$B$21:$D$21</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="3"/>
@@ -967,7 +970,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Scalability!$I$4</c:f>
+              <c:f>Scalability!$A$22</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -988,7 +991,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Scalability!$J$2:$L$2</c:f>
+              <c:f>Scalability!$B$20:$D$20</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -1005,7 +1008,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Scalability!$J$4:$L$4</c:f>
+              <c:f>Scalability!$B$22:$D$22</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="3"/>
@@ -1032,7 +1035,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Scalability!$I$5</c:f>
+              <c:f>Scalability!$A$23</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1053,7 +1056,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Scalability!$J$2:$L$2</c:f>
+              <c:f>Scalability!$B$20:$D$20</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -1070,7 +1073,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Scalability!$J$5:$L$5</c:f>
+              <c:f>Scalability!$B$23:$D$23</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="3"/>
@@ -2548,7 +2551,7 @@
           </c:marker>
           <c:yVal>
             <c:numRef>
-              <c:f>Compiler!$H$9:$K$9</c:f>
+              <c:f>Compiler!$B$9:$E$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -2960,7 +2963,7 @@
           </c:marker>
           <c:yVal>
             <c:numRef>
-              <c:f>Compiler!$H$10:$K$10</c:f>
+              <c:f>Compiler!$B$10:$E$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -3377,7 +3380,7 @@
           </c:marker>
           <c:yVal>
             <c:numRef>
-              <c:f>Compiler!$H$11:$K$11</c:f>
+              <c:f>Compiler!$B$11:$E$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -8100,16 +8103,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>138112</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>90487</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>576262</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>185737</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>538162</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>166687</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>366712</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>71437</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -8691,7 +8694,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="A2:E5"/>
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8705,9 +8708,6 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
       <c r="B2">
         <v>1</v>
       </c>
@@ -8780,10 +8780,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F135334-F4BA-43AC-A24D-8BEA4049FD5D}">
-  <dimension ref="A1:L17"/>
+  <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:A5"/>
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8794,15 +8794,12 @@
     <col min="12" max="12" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>5</v>
       </c>
-      <c r="J1" t="s">
-        <v>7</v>
-      </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -8818,17 +8815,8 @@
       <c r="E2">
         <v>4</v>
       </c>
-      <c r="J2" t="s">
-        <v>8</v>
-      </c>
-      <c r="K2" t="s">
-        <v>9</v>
-      </c>
-      <c r="L2" t="s">
-        <v>10</v>
-      </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -8844,23 +8832,8 @@
       <c r="E3">
         <v>69048</v>
       </c>
-      <c r="I3" t="s">
-        <v>2</v>
-      </c>
-      <c r="J3" s="1">
-        <f>AVERAGE(B3:E3)</f>
-        <v>56365</v>
-      </c>
-      <c r="K3" s="1">
-        <f>AVERAGE(B9:E9)</f>
-        <v>614813.75</v>
-      </c>
-      <c r="L3" s="1">
-        <f>AVERAGE(B15:E15)</f>
-        <v>6140805.75</v>
-      </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -8876,23 +8849,8 @@
       <c r="E4">
         <v>10539</v>
       </c>
-      <c r="I4" t="s">
-        <v>4</v>
-      </c>
-      <c r="J4" s="1">
-        <f>AVERAGE(B4:E4)</f>
-        <v>10641.25</v>
-      </c>
-      <c r="K4" s="1">
-        <f>AVERAGE(B10:E10)</f>
-        <v>105248.25</v>
-      </c>
-      <c r="L4" s="1">
-        <f>AVERAGE(B16:E16)</f>
-        <v>1051071.75</v>
-      </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -8908,32 +8866,17 @@
       <c r="E5">
         <v>37034</v>
       </c>
-      <c r="I5" t="s">
-        <v>3</v>
-      </c>
-      <c r="J5" s="1">
-        <f>AVERAGE(B5:E5)</f>
-        <v>37192</v>
-      </c>
-      <c r="K5" s="1">
-        <f>AVERAGE(B11:E11)</f>
-        <v>359314.5</v>
-      </c>
-      <c r="L5" s="1">
-        <f>AVERAGE(B17:E17)</f>
-        <v>3620840.5</v>
-      </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F6" s="1"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>6</v>
       </c>
       <c r="F7" s="1"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>1</v>
       </c>
@@ -8951,7 +8894,7 @@
       </c>
       <c r="F8" s="1"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>2</v>
       </c>
@@ -8968,7 +8911,7 @@
         <v>617384</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>4</v>
       </c>
@@ -8985,7 +8928,7 @@
         <v>105304</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>3</v>
       </c>
@@ -9002,16 +8945,16 @@
         <v>358631</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F12" s="1"/>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>6</v>
       </c>
       <c r="F13" s="1"/>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>1</v>
       </c>
@@ -9029,7 +8972,7 @@
       </c>
       <c r="F14" s="1"/>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>2</v>
       </c>
@@ -9046,7 +8989,7 @@
         <v>6119625</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>4</v>
       </c>
@@ -9078,6 +9021,73 @@
       </c>
       <c r="E17">
         <v>3670944</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>8</v>
+      </c>
+      <c r="C20" t="s">
+        <v>9</v>
+      </c>
+      <c r="D20" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>2</v>
+      </c>
+      <c r="B21" s="1">
+        <f>AVERAGE(B3:E3)</f>
+        <v>56365</v>
+      </c>
+      <c r="C21" s="1">
+        <f>AVERAGE(B9:E9)</f>
+        <v>614813.75</v>
+      </c>
+      <c r="D21" s="1">
+        <f>AVERAGE(B15:E15)</f>
+        <v>6140805.75</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>4</v>
+      </c>
+      <c r="B22" s="1">
+        <f>AVERAGE(B4:E4)</f>
+        <v>10641.25</v>
+      </c>
+      <c r="C22" s="1">
+        <f>AVERAGE(B10:E10)</f>
+        <v>105248.25</v>
+      </c>
+      <c r="D22" s="1">
+        <f>AVERAGE(B16:E16)</f>
+        <v>1051071.75</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>3</v>
+      </c>
+      <c r="B23" s="1">
+        <f>AVERAGE(B5:E5)</f>
+        <v>37192</v>
+      </c>
+      <c r="C23" s="1">
+        <f>AVERAGE(B11:E11)</f>
+        <v>359314.5</v>
+      </c>
+      <c r="D23" s="1">
+        <f>AVERAGE(B17:E17)</f>
+        <v>3620840.5</v>
       </c>
     </row>
   </sheetData>
@@ -9092,7 +9102,7 @@
   <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="T27" sqref="T27"/>
+      <selection activeCell="H26" sqref="H26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9409,10 +9419,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{941ACD1D-4CA7-4B34-967F-30CC36F6B77A}">
-  <dimension ref="A1:K11"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G35" sqref="G35"/>
+      <selection activeCell="M9" sqref="M9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9420,14 +9430,15 @@
     <col min="1" max="1" width="12.140625" customWidth="1"/>
     <col min="2" max="2" width="15.7109375" customWidth="1"/>
     <col min="7" max="7" width="11.85546875" customWidth="1"/>
+    <col min="8" max="8" width="12.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B2">
         <v>1</v>
       </c>
@@ -9440,8 +9451,11 @@
       <c r="E2">
         <v>4</v>
       </c>
+      <c r="I2" t="s">
+        <v>15</v>
+      </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -9457,8 +9471,19 @@
       <c r="E3">
         <v>63401</v>
       </c>
+      <c r="F3">
+        <f>AVERAGE(B3:E3)</f>
+        <v>57834</v>
+      </c>
+      <c r="H3" t="s">
+        <v>2</v>
+      </c>
+      <c r="I3">
+        <f>F9/F3*100</f>
+        <v>2.6044368364629804</v>
+      </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -9474,8 +9499,19 @@
       <c r="E4">
         <v>16049</v>
       </c>
+      <c r="F4">
+        <f>AVERAGE(B4:E4)</f>
+        <v>15188.75</v>
+      </c>
+      <c r="H4" t="s">
+        <v>4</v>
+      </c>
+      <c r="I4">
+        <f t="shared" ref="I4:I5" si="0">F10/F4*100</f>
+        <v>2.1216360793350342</v>
+      </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -9491,75 +9527,98 @@
       <c r="E5">
         <v>38064</v>
       </c>
+      <c r="F5">
+        <f>AVERAGE(B5:E5)</f>
+        <v>40540</v>
+      </c>
+      <c r="H5" t="s">
+        <v>3</v>
+      </c>
+      <c r="I5">
+        <f t="shared" si="0"/>
+        <v>10.128268376911691</v>
+      </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="H7" t="s">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="H8">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B8">
         <v>1</v>
       </c>
-      <c r="I8">
+      <c r="C8">
         <v>2</v>
       </c>
-      <c r="J8">
+      <c r="D8">
         <v>3</v>
       </c>
-      <c r="K8">
+      <c r="E8">
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="G9" t="s">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>2</v>
       </c>
-      <c r="H9">
+      <c r="B9">
         <v>1698</v>
       </c>
-      <c r="I9">
+      <c r="C9">
         <v>1371</v>
       </c>
-      <c r="J9">
+      <c r="D9">
         <v>1210</v>
       </c>
-      <c r="K9">
+      <c r="E9">
         <v>1746</v>
       </c>
+      <c r="F9">
+        <f>AVERAGE(B9:E9)</f>
+        <v>1506.25</v>
+      </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="G10" t="s">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>4</v>
       </c>
-      <c r="H10">
+      <c r="B10">
         <v>284</v>
       </c>
-      <c r="I10">
+      <c r="C10">
         <v>270</v>
       </c>
-      <c r="J10">
+      <c r="D10">
         <v>268</v>
       </c>
-      <c r="K10">
+      <c r="E10">
         <v>467</v>
       </c>
+      <c r="F10">
+        <f>AVERAGE(B10:E10)</f>
+        <v>322.25</v>
+      </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="G11" t="s">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>3</v>
       </c>
-      <c r="H11">
+      <c r="B11">
         <v>4165</v>
       </c>
-      <c r="I11">
+      <c r="C11">
         <v>4226</v>
       </c>
-      <c r="J11">
+      <c r="D11">
         <v>3870</v>
       </c>
-      <c r="K11">
+      <c r="E11">
         <v>4163</v>
+      </c>
+      <c r="F11">
+        <f>AVERAGE(B11:E11)</f>
+        <v>4106</v>
       </c>
     </row>
   </sheetData>

</xml_diff>